<commit_message>
2023-11-03 01:22:15 - nameAccentsUpdate in excel
</commit_message>
<xml_diff>
--- a/output/output.xlsx
+++ b/output/output.xlsx
@@ -468,7 +468,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Aidan McCarron MCIOB</t>
+          <t>Aidan Mc</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -492,7 +492,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>John Higgins MCIOB</t>
+          <t>John Higgins</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -502,7 +502,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Higgins MCIOB</t>
+          <t>Higgins</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -516,7 +516,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Michael Yohanis MCIOB</t>
+          <t>Michael Yohanis</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -526,7 +526,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Yohanis MCIOB</t>
+          <t>Yohanis</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -540,7 +540,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Declan McLogan CMIOSH LL.M</t>
+          <t>Declan Mc</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -550,7 +550,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>McLogan CMIOSH LL.M</t>
+          <t>Mc</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -676,17 +676,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Lee Robert Gray GradIOSH</t>
+          <t>Lee Robert Gray Grad</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Lee Robert </t>
+          <t>Lee Robert</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Gray GradIOSH</t>
+          <t>Gray Grad</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -708,7 +708,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Eamonn Laverty. MCIOB</t>
+          <t>Eamonn Laverty</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -718,7 +718,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Laverty. MCIOB</t>
+          <t>Laverty</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -804,17 +804,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Sinéad Gorman (she/her)</t>
+          <t>Sinead Gorman</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Sinéad</t>
+          <t>Sinead</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Gorman (she/her)</t>
+          <t>Gorman</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -924,7 +924,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Nina Salandy    BSc. (Hons.) GradIOSH</t>
+          <t>Nina Salandy</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -934,7 +934,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Salandy    BSc. (Hons.) GradIOSH</t>
+          <t>Salandy</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">

</xml_diff>

<commit_message>
2023-11-05 04:18:01 - done with renaming
</commit_message>
<xml_diff>
--- a/output/output.xlsx
+++ b/output/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,10 +456,20 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Phones</t>
+          <t>Title</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Country</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Phone</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Emails</t>
         </is>
@@ -486,8 +496,18 @@
           <t>McAleer &amp; Rushe</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Project Director</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>United Kingdom</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -510,8 +530,18 @@
           <t>McAleer &amp; Rushe</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Project Director</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Cookstown, Northern Ireland, United Kingdom</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -534,8 +564,18 @@
           <t>McAleer &amp; Rushe</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Project Director</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Belfast</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -558,8 +598,18 @@
           <t>McAleer &amp; Rushe</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Director of SHEQ</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Cookstown</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -584,10 +634,20 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
+          <t>Project Director</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>London, England, United Kingdom</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
           <t>+44 7826 532410</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>lorcan.mulvey@mcaleer-rushe.co.uk , lorcanmulvey@yahoo.ie , lorcan.mulvey@yahoo.ie , lorcan.mulvey@berkeleygroup.co.uk</t>
         </is>
@@ -614,8 +674,18 @@
           <t>McAleer &amp; Rushe</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Project Manager</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>London, England, United Kingdom</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -640,10 +710,20 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
+          <t>Contracts Director</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>London, United Kingdom</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
           <t>+44 7912 046630</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="H8" t="inlineStr">
         <is>
           <t>darragh.greenan@mcaleer-rushe.co.uk</t>
         </is>
@@ -670,8 +750,18 @@
           <t>McAleer &amp; Rushe</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Project Director</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Belfast Metropolitan Area</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -696,10 +786,20 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
+          <t>Senior SHEQ Advisor</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Newcastle upon Tyne, England, United Kingdom</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
           <t>07872331053</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="H10" t="inlineStr">
         <is>
           <t>leergray3@hotmail.co.uk , lee.gray@mcaleer-rushe.co.uk</t>
         </is>
@@ -726,8 +826,18 @@
           <t>Thornton Roofing</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Construction Operations Manager</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Ireland</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -750,8 +860,18 @@
           <t>McAleer &amp; Rushe</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Project Director</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>London Area, United Kingdom</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -774,8 +894,18 @@
           <t>McAleer &amp; Rushe</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Project Manager</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Belfast, Northern Ireland, United Kingdom</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -798,8 +928,18 @@
           <t>McAleer &amp; Rushe</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Assistant Project Manager</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>London, England, United Kingdom</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -822,8 +962,18 @@
           <t>McAleer &amp; Rushe</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>SHEQ Officer</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Belfast, United Kingdom</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -848,10 +998,20 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
+          <t>Head of Buying</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Cookstown, N.Ireland</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
           <t>+44 28 2565 0003</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="H16" t="inlineStr">
         <is>
           <t>connor.graham@patton.co.uk , connor.graham@mcaleer-rushe.co.uk</t>
         </is>
@@ -880,10 +1040,20 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
+          <t>Health and Safety Officer</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>London, United Kingdom</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
           <t>+44 7835 631685</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="H17" t="inlineStr">
         <is>
           <t>cathal.magee@mcaleer-rushe.co.uk , cathal.magee1@hotmail.co.uk</t>
         </is>
@@ -912,10 +1082,20 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
+          <t>M&amp;E</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Cookstown</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
           <t>+55 21 98139-3298 , +55 92 98855-0059 , +55 92 98802-4114</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="H18" t="inlineStr">
         <is>
           <t>bruno.antoniazzi@mcaleer-rushe.co.uk</t>
         </is>
@@ -942,8 +1122,18 @@
           <t>McAleer &amp; Rushe</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Snr. SHEQ Advisor</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>London, England, United Kingdom</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -966,8 +1156,18 @@
           <t>McAleer &amp; Rushe</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr"/>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Senior Construction Manager</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Belfast, United Kingdom</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -990,8 +1190,18 @@
           <t>McAleer &amp; Rushe</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr"/>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Project Manager</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Cookstown, Northern Ireland, United Kingdom</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1014,8 +1224,18 @@
           <t>McAleer &amp; Rushe</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr"/>
-      <c r="F22" t="inlineStr"/>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Health and safety administrator</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Wembley, England, United Kingdom</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
2023-11-05 13:18:16 - Working Docker Module
</commit_message>
<xml_diff>
--- a/output/output.xlsx
+++ b/output/output.xlsx
@@ -471,7 +471,7 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Emails</t>
+          <t>Email</t>
         </is>
       </c>
     </row>
@@ -507,7 +507,11 @@
         </is>
       </c>
       <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>aidan.mccarron@mcaleer-rushe.co.uk</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -541,7 +545,11 @@
         </is>
       </c>
       <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>john.higgins@mcaleer-rushe.co.uk</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -575,7 +583,11 @@
         </is>
       </c>
       <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>michael.yohanis@mcaleer-rushe.co.uk</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -609,7 +621,11 @@
         </is>
       </c>
       <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>declan.mc@mcaleer-rushe.co.uk</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -649,7 +665,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>lorcan.mulvey@mcaleer-rushe.co.uk , lorcanmulvey@yahoo.ie , lorcan.mulvey@yahoo.ie , lorcan.mulvey@berkeleygroup.co.uk</t>
+          <t>lorcan.mulvey@mcaleer-rushe.co.uk</t>
         </is>
       </c>
     </row>
@@ -685,7 +701,11 @@
         </is>
       </c>
       <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>gerald.laverty@mcaleer-rushe.co.uk</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -761,7 +781,11 @@
         </is>
       </c>
       <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>steve.morris@mcaleer-rushe.co.uk</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -801,7 +825,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>leergray3@hotmail.co.uk , lee.gray@mcaleer-rushe.co.uk</t>
+          <t>lee.gray@mcaleer-rushe.co.uk</t>
         </is>
       </c>
     </row>
@@ -837,7 +861,11 @@
         </is>
       </c>
       <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>eamonn.laverty@thorntonroofing.com</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -871,7 +899,11 @@
         </is>
       </c>
       <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>eoin.gormley@mcaleer-rushe.co.uk</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -905,7 +937,11 @@
         </is>
       </c>
       <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>paddy.connolly@mcaleer-rushe.co.uk</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -939,7 +975,11 @@
         </is>
       </c>
       <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>daisy.butterworth@mcaleer-rushe.co.uk</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -973,7 +1013,11 @@
         </is>
       </c>
       <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>sinead.gorman@mcaleer-rushe.co.uk</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1013,7 +1057,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>connor.graham@patton.co.uk , connor.graham@mcaleer-rushe.co.uk</t>
+          <t>connor.graham@mcaleer-rushe.co.uk</t>
         </is>
       </c>
     </row>
@@ -1055,7 +1099,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>cathal.magee@mcaleer-rushe.co.uk , cathal.magee1@hotmail.co.uk</t>
+          <t>cathal.magee@mcaleer-rushe.co.uk</t>
         </is>
       </c>
     </row>
@@ -1133,7 +1177,11 @@
         </is>
       </c>
       <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr"/>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>nina.salandy@mcaleer-rushe.co.uk</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1167,7 +1215,11 @@
         </is>
       </c>
       <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr"/>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>peter.coyle@mcaleer-rushe.co.uk</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1201,7 +1253,11 @@
         </is>
       </c>
       <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr"/>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>orran.devine@mcaleer-rushe.co.uk</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1235,7 +1291,11 @@
         </is>
       </c>
       <c r="G22" t="inlineStr"/>
-      <c r="H22" t="inlineStr"/>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>niamh.heneghan@mcaleer-rushe.co.uk</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>